<commit_message>
Upload experimental excel data
</commit_message>
<xml_diff>
--- a/ExperimentalData/StepResponse_1.xlsx
+++ b/ExperimentalData/StepResponse_1.xlsx
@@ -783,11 +783,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="409765352"/>
-        <c:axId val="409764568"/>
+        <c:axId val="407152136"/>
+        <c:axId val="407156056"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="409765352"/>
+        <c:axId val="407152136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -900,12 +900,12 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="409764568"/>
+        <c:crossAx val="407156056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="409764568"/>
+        <c:axId val="407156056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1030,7 +1030,667 @@
             <a:endParaRPr lang="zh-TW"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="409765352"/>
+        <c:crossAx val="407152136"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-TW"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA" altLang="zh-TW"/>
+              <a:t>Step Response</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-CA" altLang="zh-TW" baseline="0"/>
+              <a:t> (Need more measurement)</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-CA" altLang="zh-TW"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="zh-TW"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Sheet1!$O$13:$O$71</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="59"/>
+                <c:pt idx="0">
+                  <c:v>227</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>287</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>348</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>408</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>469</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>530</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>590</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>652</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>712</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>772</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>833</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>893</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>955</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1015</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1076</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1137</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1197</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1258</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1319</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1380</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1440</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1502</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1562</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>1622</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1684</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1744</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>1805</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1866</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1927</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1988</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>2048</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>2109</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2169</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>2231</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2291</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2351</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2413</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>2473</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>2534</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2595</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>2656</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>2717</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>2777</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2838</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2899</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2960</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>3020</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>3082</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>3142</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>3202</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>3264</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>3324</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>3385</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>3446</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>3507</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>3567</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>3627</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>3689</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>3749</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Sheet1!$P$13:$P$71</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="59"/>
+                <c:pt idx="0">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>52</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>78</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>76</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>118</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>154</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>162</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>134</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>152</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>126</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>158</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>154</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>162</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>154</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>162</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>158</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>154</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>166</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>182</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>172</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>150</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>158</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>170</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>174</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>166</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>156</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>156</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>160</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>148</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>124</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>122</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>114</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="410562328"/>
+        <c:axId val="410570952"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="410562328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-TW"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="410570952"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="410570952"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-TW"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="410562328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1119,6 +1779,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -1635,20 +2335,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>295274</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>171449</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>609599</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:colOff>485774</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1667,15 +2883,45 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>476250</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PositionTimeMotor_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PositionTimeMotor" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PositionTimeMotor" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PositionTimeMotor_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1941,10 +3187,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:L72"/>
+  <dimension ref="B4:P72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13:P71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -1955,7 +3201,7 @@
     <col min="9" max="9" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:12">
+    <row r="4" spans="2:16">
       <c r="B4">
         <v>404</v>
       </c>
@@ -1963,7 +3209,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="5" spans="2:12">
+    <row r="5" spans="2:16">
       <c r="B5">
         <v>1306</v>
       </c>
@@ -1971,7 +3217,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="6" spans="2:12">
+    <row r="6" spans="2:16">
       <c r="B6">
         <v>2266</v>
       </c>
@@ -1979,7 +3225,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="7" spans="2:12">
+    <row r="7" spans="2:16">
       <c r="B7">
         <v>3234</v>
       </c>
@@ -1987,7 +3233,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="8" spans="2:12">
+    <row r="8" spans="2:16">
       <c r="B8">
         <v>4225</v>
       </c>
@@ -1995,7 +3241,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="9" spans="2:12">
+    <row r="9" spans="2:16">
       <c r="B9">
         <v>5249</v>
       </c>
@@ -2003,7 +3249,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="10" spans="2:12">
+    <row r="10" spans="2:16">
       <c r="B10">
         <v>6290</v>
       </c>
@@ -2011,7 +3257,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="11" spans="2:12">
+    <row r="11" spans="2:16">
       <c r="B11">
         <v>7356</v>
       </c>
@@ -2019,7 +3265,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="12" spans="2:12">
+    <row r="12" spans="2:16">
       <c r="B12">
         <v>8430</v>
       </c>
@@ -2027,7 +3273,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="13" spans="2:12">
+    <row r="13" spans="2:16">
       <c r="B13">
         <v>9518</v>
       </c>
@@ -2051,8 +3297,20 @@
         <f>I13-1000</f>
         <v>227</v>
       </c>
-    </row>
-    <row r="14" spans="2:12">
+      <c r="N13">
+        <f>K14-K13</f>
+        <v>4</v>
+      </c>
+      <c r="O13">
+        <f>L13</f>
+        <v>227</v>
+      </c>
+      <c r="P13">
+        <f>N13</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="2:16">
       <c r="B14">
         <v>10614</v>
       </c>
@@ -2076,8 +3334,20 @@
         <f t="shared" ref="L14:L72" si="1">I14-1000</f>
         <v>287</v>
       </c>
-    </row>
-    <row r="15" spans="2:12">
+      <c r="N14">
+        <f t="shared" ref="N14:N72" si="2">K15-K14</f>
+        <v>52</v>
+      </c>
+      <c r="O14">
+        <f t="shared" ref="O14:O71" si="3">L14</f>
+        <v>287</v>
+      </c>
+      <c r="P14">
+        <f t="shared" ref="P14:P71" si="4">N14</f>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="15" spans="2:16">
       <c r="B15">
         <v>11720</v>
       </c>
@@ -2101,8 +3371,20 @@
         <f t="shared" si="1"/>
         <v>348</v>
       </c>
-    </row>
-    <row r="16" spans="2:12">
+      <c r="N15">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="3"/>
+        <v>348</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="4"/>
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="2:16">
       <c r="B16">
         <v>12824</v>
       </c>
@@ -2126,8 +3408,20 @@
         <f t="shared" si="1"/>
         <v>408</v>
       </c>
-    </row>
-    <row r="17" spans="2:12">
+      <c r="N16">
+        <f t="shared" si="2"/>
+        <v>94</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="3"/>
+        <v>408</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="4"/>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16">
       <c r="B17">
         <v>13918</v>
       </c>
@@ -2151,8 +3445,20 @@
         <f t="shared" si="1"/>
         <v>469</v>
       </c>
-    </row>
-    <row r="18" spans="2:12">
+      <c r="N17">
+        <f t="shared" si="2"/>
+        <v>80</v>
+      </c>
+      <c r="O17">
+        <f t="shared" si="3"/>
+        <v>469</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="4"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16">
       <c r="B18">
         <v>15016</v>
       </c>
@@ -2176,8 +3482,20 @@
         <f t="shared" si="1"/>
         <v>530</v>
       </c>
-    </row>
-    <row r="19" spans="2:12">
+      <c r="N18">
+        <f t="shared" si="2"/>
+        <v>94</v>
+      </c>
+      <c r="O18">
+        <f t="shared" si="3"/>
+        <v>530</v>
+      </c>
+      <c r="P18">
+        <f t="shared" si="4"/>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16">
       <c r="B19">
         <v>16120</v>
       </c>
@@ -2201,8 +3519,20 @@
         <f t="shared" si="1"/>
         <v>590</v>
       </c>
-    </row>
-    <row r="20" spans="2:12">
+      <c r="N19">
+        <f t="shared" si="2"/>
+        <v>78</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="3"/>
+        <v>590</v>
+      </c>
+      <c r="P19">
+        <f t="shared" si="4"/>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16">
       <c r="B20">
         <v>17222</v>
       </c>
@@ -2226,8 +3556,20 @@
         <f t="shared" si="1"/>
         <v>652</v>
       </c>
-    </row>
-    <row r="21" spans="2:12">
+      <c r="N20">
+        <f t="shared" si="2"/>
+        <v>76</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="3"/>
+        <v>652</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="4"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16">
       <c r="B21">
         <v>18320</v>
       </c>
@@ -2251,8 +3593,20 @@
         <f t="shared" si="1"/>
         <v>712</v>
       </c>
-    </row>
-    <row r="22" spans="2:12">
+      <c r="N21">
+        <f t="shared" si="2"/>
+        <v>108</v>
+      </c>
+      <c r="O21">
+        <f t="shared" si="3"/>
+        <v>712</v>
+      </c>
+      <c r="P21">
+        <f t="shared" si="4"/>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16">
       <c r="B22">
         <v>19422</v>
       </c>
@@ -2276,8 +3630,20 @@
         <f t="shared" si="1"/>
         <v>772</v>
       </c>
-    </row>
-    <row r="23" spans="2:12">
+      <c r="N22">
+        <f t="shared" si="2"/>
+        <v>106</v>
+      </c>
+      <c r="O22">
+        <f t="shared" si="3"/>
+        <v>772</v>
+      </c>
+      <c r="P22">
+        <f t="shared" si="4"/>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16">
       <c r="B23">
         <v>20526</v>
       </c>
@@ -2301,8 +3667,20 @@
         <f t="shared" si="1"/>
         <v>833</v>
       </c>
-    </row>
-    <row r="24" spans="2:12">
+      <c r="N23">
+        <f t="shared" si="2"/>
+        <v>132</v>
+      </c>
+      <c r="O23">
+        <f t="shared" si="3"/>
+        <v>833</v>
+      </c>
+      <c r="P23">
+        <f t="shared" si="4"/>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16">
       <c r="B24">
         <v>21618</v>
       </c>
@@ -2326,8 +3704,20 @@
         <f t="shared" si="1"/>
         <v>893</v>
       </c>
-    </row>
-    <row r="25" spans="2:12">
+      <c r="N24">
+        <f t="shared" si="2"/>
+        <v>138</v>
+      </c>
+      <c r="O24">
+        <f t="shared" si="3"/>
+        <v>893</v>
+      </c>
+      <c r="P24">
+        <f t="shared" si="4"/>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16">
       <c r="B25">
         <v>22714</v>
       </c>
@@ -2351,8 +3741,20 @@
         <f t="shared" si="1"/>
         <v>955</v>
       </c>
-    </row>
-    <row r="26" spans="2:12">
+      <c r="N25">
+        <f t="shared" si="2"/>
+        <v>118</v>
+      </c>
+      <c r="O25">
+        <f t="shared" si="3"/>
+        <v>955</v>
+      </c>
+      <c r="P25">
+        <f t="shared" si="4"/>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16">
       <c r="B26">
         <v>23810</v>
       </c>
@@ -2376,8 +3778,20 @@
         <f t="shared" si="1"/>
         <v>1015</v>
       </c>
-    </row>
-    <row r="27" spans="2:12">
+      <c r="N26">
+        <f t="shared" si="2"/>
+        <v>132</v>
+      </c>
+      <c r="O26">
+        <f t="shared" si="3"/>
+        <v>1015</v>
+      </c>
+      <c r="P26">
+        <f t="shared" si="4"/>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16">
       <c r="B27">
         <v>24900</v>
       </c>
@@ -2401,8 +3815,20 @@
         <f t="shared" si="1"/>
         <v>1076</v>
       </c>
-    </row>
-    <row r="28" spans="2:12">
+      <c r="N27">
+        <f t="shared" si="2"/>
+        <v>146</v>
+      </c>
+      <c r="O27">
+        <f t="shared" si="3"/>
+        <v>1076</v>
+      </c>
+      <c r="P27">
+        <f t="shared" si="4"/>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16">
       <c r="B28">
         <v>25970</v>
       </c>
@@ -2426,8 +3852,20 @@
         <f t="shared" si="1"/>
         <v>1137</v>
       </c>
-    </row>
-    <row r="29" spans="2:12">
+      <c r="N28">
+        <f t="shared" si="2"/>
+        <v>154</v>
+      </c>
+      <c r="O28">
+        <f t="shared" si="3"/>
+        <v>1137</v>
+      </c>
+      <c r="P28">
+        <f t="shared" si="4"/>
+        <v>154</v>
+      </c>
+    </row>
+    <row r="29" spans="2:16">
       <c r="B29">
         <v>27054</v>
       </c>
@@ -2451,8 +3889,20 @@
         <f t="shared" si="1"/>
         <v>1197</v>
       </c>
-    </row>
-    <row r="30" spans="2:12">
+      <c r="N29">
+        <f t="shared" si="2"/>
+        <v>162</v>
+      </c>
+      <c r="O29">
+        <f t="shared" si="3"/>
+        <v>1197</v>
+      </c>
+      <c r="P29">
+        <f t="shared" si="4"/>
+        <v>162</v>
+      </c>
+    </row>
+    <row r="30" spans="2:16">
       <c r="B30">
         <v>28146</v>
       </c>
@@ -2476,8 +3926,20 @@
         <f t="shared" si="1"/>
         <v>1258</v>
       </c>
-    </row>
-    <row r="31" spans="2:12">
+      <c r="N30">
+        <f t="shared" si="2"/>
+        <v>132</v>
+      </c>
+      <c r="O30">
+        <f t="shared" si="3"/>
+        <v>1258</v>
+      </c>
+      <c r="P30">
+        <f t="shared" si="4"/>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="31" spans="2:16">
       <c r="B31">
         <v>29250</v>
       </c>
@@ -2501,8 +3963,20 @@
         <f t="shared" si="1"/>
         <v>1319</v>
       </c>
-    </row>
-    <row r="32" spans="2:12">
+      <c r="N31">
+        <f t="shared" si="2"/>
+        <v>120</v>
+      </c>
+      <c r="O31">
+        <f t="shared" si="3"/>
+        <v>1319</v>
+      </c>
+      <c r="P31">
+        <f t="shared" si="4"/>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="32" spans="2:16">
       <c r="B32">
         <v>30356</v>
       </c>
@@ -2526,8 +4000,20 @@
         <f t="shared" si="1"/>
         <v>1380</v>
       </c>
-    </row>
-    <row r="33" spans="2:12">
+      <c r="N32">
+        <f t="shared" si="2"/>
+        <v>134</v>
+      </c>
+      <c r="O32">
+        <f t="shared" si="3"/>
+        <v>1380</v>
+      </c>
+      <c r="P32">
+        <f t="shared" si="4"/>
+        <v>134</v>
+      </c>
+    </row>
+    <row r="33" spans="2:16">
       <c r="B33">
         <v>31454</v>
       </c>
@@ -2551,8 +4037,20 @@
         <f t="shared" si="1"/>
         <v>1440</v>
       </c>
-    </row>
-    <row r="34" spans="2:12">
+      <c r="N33">
+        <f t="shared" si="2"/>
+        <v>130</v>
+      </c>
+      <c r="O33">
+        <f t="shared" si="3"/>
+        <v>1440</v>
+      </c>
+      <c r="P33">
+        <f t="shared" si="4"/>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="34" spans="2:16">
       <c r="B34">
         <v>32548</v>
       </c>
@@ -2576,8 +4074,20 @@
         <f t="shared" si="1"/>
         <v>1502</v>
       </c>
-    </row>
-    <row r="35" spans="2:12">
+      <c r="N34">
+        <f t="shared" si="2"/>
+        <v>152</v>
+      </c>
+      <c r="O34">
+        <f t="shared" si="3"/>
+        <v>1502</v>
+      </c>
+      <c r="P34">
+        <f t="shared" si="4"/>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="35" spans="2:16">
       <c r="F35" t="s">
         <v>22</v>
       </c>
@@ -2595,8 +4105,20 @@
         <f t="shared" si="1"/>
         <v>1562</v>
       </c>
-    </row>
-    <row r="36" spans="2:12">
+      <c r="N35">
+        <f t="shared" si="2"/>
+        <v>120</v>
+      </c>
+      <c r="O35">
+        <f t="shared" si="3"/>
+        <v>1562</v>
+      </c>
+      <c r="P35">
+        <f t="shared" si="4"/>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="36" spans="2:16">
       <c r="F36" t="s">
         <v>23</v>
       </c>
@@ -2614,8 +4136,20 @@
         <f t="shared" si="1"/>
         <v>1622</v>
       </c>
-    </row>
-    <row r="37" spans="2:12">
+      <c r="N36">
+        <f t="shared" si="2"/>
+        <v>114</v>
+      </c>
+      <c r="O36">
+        <f t="shared" si="3"/>
+        <v>1622</v>
+      </c>
+      <c r="P36">
+        <f t="shared" si="4"/>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="37" spans="2:16">
       <c r="F37" t="s">
         <v>24</v>
       </c>
@@ -2633,8 +4167,20 @@
         <f t="shared" si="1"/>
         <v>1684</v>
       </c>
-    </row>
-    <row r="38" spans="2:12">
+      <c r="N37">
+        <f t="shared" si="2"/>
+        <v>110</v>
+      </c>
+      <c r="O37">
+        <f t="shared" si="3"/>
+        <v>1684</v>
+      </c>
+      <c r="P37">
+        <f t="shared" si="4"/>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="38" spans="2:16">
       <c r="F38" t="s">
         <v>25</v>
       </c>
@@ -2652,8 +4198,20 @@
         <f t="shared" si="1"/>
         <v>1744</v>
       </c>
-    </row>
-    <row r="39" spans="2:12">
+      <c r="N38">
+        <f t="shared" si="2"/>
+        <v>126</v>
+      </c>
+      <c r="O38">
+        <f t="shared" si="3"/>
+        <v>1744</v>
+      </c>
+      <c r="P38">
+        <f t="shared" si="4"/>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="39" spans="2:16">
       <c r="F39" t="s">
         <v>26</v>
       </c>
@@ -2671,8 +4229,20 @@
         <f t="shared" si="1"/>
         <v>1805</v>
       </c>
-    </row>
-    <row r="40" spans="2:12">
+      <c r="N39">
+        <f t="shared" si="2"/>
+        <v>150</v>
+      </c>
+      <c r="O39">
+        <f t="shared" si="3"/>
+        <v>1805</v>
+      </c>
+      <c r="P39">
+        <f t="shared" si="4"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="40" spans="2:16">
       <c r="F40" t="s">
         <v>27</v>
       </c>
@@ -2690,8 +4260,20 @@
         <f t="shared" si="1"/>
         <v>1866</v>
       </c>
-    </row>
-    <row r="41" spans="2:12">
+      <c r="N40">
+        <f t="shared" si="2"/>
+        <v>150</v>
+      </c>
+      <c r="O40">
+        <f t="shared" si="3"/>
+        <v>1866</v>
+      </c>
+      <c r="P40">
+        <f t="shared" si="4"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="41" spans="2:16">
       <c r="F41" t="s">
         <v>28</v>
       </c>
@@ -2709,8 +4291,20 @@
         <f t="shared" si="1"/>
         <v>1927</v>
       </c>
-    </row>
-    <row r="42" spans="2:12">
+      <c r="N41">
+        <f t="shared" si="2"/>
+        <v>158</v>
+      </c>
+      <c r="O41">
+        <f t="shared" si="3"/>
+        <v>1927</v>
+      </c>
+      <c r="P41">
+        <f t="shared" si="4"/>
+        <v>158</v>
+      </c>
+    </row>
+    <row r="42" spans="2:16">
       <c r="F42" t="s">
         <v>29</v>
       </c>
@@ -2728,8 +4322,20 @@
         <f t="shared" si="1"/>
         <v>1988</v>
       </c>
-    </row>
-    <row r="43" spans="2:12">
+      <c r="N42">
+        <f t="shared" si="2"/>
+        <v>154</v>
+      </c>
+      <c r="O42">
+        <f t="shared" si="3"/>
+        <v>1988</v>
+      </c>
+      <c r="P42">
+        <f t="shared" si="4"/>
+        <v>154</v>
+      </c>
+    </row>
+    <row r="43" spans="2:16">
       <c r="F43" t="s">
         <v>30</v>
       </c>
@@ -2747,8 +4353,20 @@
         <f t="shared" si="1"/>
         <v>2048</v>
       </c>
-    </row>
-    <row r="44" spans="2:12">
+      <c r="N43">
+        <f t="shared" si="2"/>
+        <v>162</v>
+      </c>
+      <c r="O43">
+        <f t="shared" si="3"/>
+        <v>2048</v>
+      </c>
+      <c r="P43">
+        <f t="shared" si="4"/>
+        <v>162</v>
+      </c>
+    </row>
+    <row r="44" spans="2:16">
       <c r="F44" t="s">
         <v>31</v>
       </c>
@@ -2766,8 +4384,20 @@
         <f t="shared" si="1"/>
         <v>2109</v>
       </c>
-    </row>
-    <row r="45" spans="2:12">
+      <c r="N44">
+        <f t="shared" si="2"/>
+        <v>154</v>
+      </c>
+      <c r="O44">
+        <f t="shared" si="3"/>
+        <v>2109</v>
+      </c>
+      <c r="P44">
+        <f t="shared" si="4"/>
+        <v>154</v>
+      </c>
+    </row>
+    <row r="45" spans="2:16">
       <c r="F45" t="s">
         <v>32</v>
       </c>
@@ -2785,8 +4415,20 @@
         <f t="shared" si="1"/>
         <v>2169</v>
       </c>
-    </row>
-    <row r="46" spans="2:12">
+      <c r="N45">
+        <f t="shared" si="2"/>
+        <v>170</v>
+      </c>
+      <c r="O45">
+        <f t="shared" si="3"/>
+        <v>2169</v>
+      </c>
+      <c r="P45">
+        <f t="shared" si="4"/>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="46" spans="2:16">
       <c r="F46" t="s">
         <v>33</v>
       </c>
@@ -2804,8 +4446,20 @@
         <f t="shared" si="1"/>
         <v>2231</v>
       </c>
-    </row>
-    <row r="47" spans="2:12">
+      <c r="N46">
+        <f t="shared" si="2"/>
+        <v>162</v>
+      </c>
+      <c r="O46">
+        <f t="shared" si="3"/>
+        <v>2231</v>
+      </c>
+      <c r="P46">
+        <f t="shared" si="4"/>
+        <v>162</v>
+      </c>
+    </row>
+    <row r="47" spans="2:16">
       <c r="F47" t="s">
         <v>34</v>
       </c>
@@ -2823,8 +4477,20 @@
         <f t="shared" si="1"/>
         <v>2291</v>
       </c>
-    </row>
-    <row r="48" spans="2:12">
+      <c r="N47">
+        <f t="shared" si="2"/>
+        <v>158</v>
+      </c>
+      <c r="O47">
+        <f t="shared" si="3"/>
+        <v>2291</v>
+      </c>
+      <c r="P47">
+        <f t="shared" si="4"/>
+        <v>158</v>
+      </c>
+    </row>
+    <row r="48" spans="2:16">
       <c r="F48" t="s">
         <v>35</v>
       </c>
@@ -2842,8 +4508,20 @@
         <f t="shared" si="1"/>
         <v>2351</v>
       </c>
-    </row>
-    <row r="49" spans="6:12">
+      <c r="N48">
+        <f t="shared" si="2"/>
+        <v>154</v>
+      </c>
+      <c r="O48">
+        <f t="shared" si="3"/>
+        <v>2351</v>
+      </c>
+      <c r="P48">
+        <f t="shared" si="4"/>
+        <v>154</v>
+      </c>
+    </row>
+    <row r="49" spans="6:16">
       <c r="F49" t="s">
         <v>36</v>
       </c>
@@ -2861,8 +4539,20 @@
         <f t="shared" si="1"/>
         <v>2413</v>
       </c>
-    </row>
-    <row r="50" spans="6:12">
+      <c r="N49">
+        <f t="shared" si="2"/>
+        <v>166</v>
+      </c>
+      <c r="O49">
+        <f t="shared" si="3"/>
+        <v>2413</v>
+      </c>
+      <c r="P49">
+        <f t="shared" si="4"/>
+        <v>166</v>
+      </c>
+    </row>
+    <row r="50" spans="6:16">
       <c r="F50" t="s">
         <v>37</v>
       </c>
@@ -2880,8 +4570,20 @@
         <f t="shared" si="1"/>
         <v>2473</v>
       </c>
-    </row>
-    <row r="51" spans="6:12">
+      <c r="N50">
+        <f t="shared" si="2"/>
+        <v>182</v>
+      </c>
+      <c r="O50">
+        <f t="shared" si="3"/>
+        <v>2473</v>
+      </c>
+      <c r="P50">
+        <f t="shared" si="4"/>
+        <v>182</v>
+      </c>
+    </row>
+    <row r="51" spans="6:16">
       <c r="F51" t="s">
         <v>38</v>
       </c>
@@ -2899,8 +4601,20 @@
         <f t="shared" si="1"/>
         <v>2534</v>
       </c>
-    </row>
-    <row r="52" spans="6:12">
+      <c r="N51">
+        <f t="shared" si="2"/>
+        <v>172</v>
+      </c>
+      <c r="O51">
+        <f t="shared" si="3"/>
+        <v>2534</v>
+      </c>
+      <c r="P51">
+        <f t="shared" si="4"/>
+        <v>172</v>
+      </c>
+    </row>
+    <row r="52" spans="6:16">
       <c r="F52" t="s">
         <v>39</v>
       </c>
@@ -2918,8 +4632,20 @@
         <f t="shared" si="1"/>
         <v>2595</v>
       </c>
-    </row>
-    <row r="53" spans="6:12">
+      <c r="N52">
+        <f t="shared" si="2"/>
+        <v>150</v>
+      </c>
+      <c r="O52">
+        <f t="shared" si="3"/>
+        <v>2595</v>
+      </c>
+      <c r="P52">
+        <f t="shared" si="4"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="53" spans="6:16">
       <c r="F53" t="s">
         <v>40</v>
       </c>
@@ -2937,8 +4663,20 @@
         <f t="shared" si="1"/>
         <v>2656</v>
       </c>
-    </row>
-    <row r="54" spans="6:12">
+      <c r="N53">
+        <f t="shared" si="2"/>
+        <v>158</v>
+      </c>
+      <c r="O53">
+        <f t="shared" si="3"/>
+        <v>2656</v>
+      </c>
+      <c r="P53">
+        <f t="shared" si="4"/>
+        <v>158</v>
+      </c>
+    </row>
+    <row r="54" spans="6:16">
       <c r="F54" t="s">
         <v>41</v>
       </c>
@@ -2956,8 +4694,20 @@
         <f t="shared" si="1"/>
         <v>2717</v>
       </c>
-    </row>
-    <row r="55" spans="6:12">
+      <c r="N54">
+        <f t="shared" si="2"/>
+        <v>170</v>
+      </c>
+      <c r="O54">
+        <f t="shared" si="3"/>
+        <v>2717</v>
+      </c>
+      <c r="P54">
+        <f t="shared" si="4"/>
+        <v>170</v>
+      </c>
+    </row>
+    <row r="55" spans="6:16">
       <c r="F55" t="s">
         <v>42</v>
       </c>
@@ -2975,8 +4725,20 @@
         <f t="shared" si="1"/>
         <v>2777</v>
       </c>
-    </row>
-    <row r="56" spans="6:12">
+      <c r="N55">
+        <f t="shared" si="2"/>
+        <v>174</v>
+      </c>
+      <c r="O55">
+        <f t="shared" si="3"/>
+        <v>2777</v>
+      </c>
+      <c r="P55">
+        <f t="shared" si="4"/>
+        <v>174</v>
+      </c>
+    </row>
+    <row r="56" spans="6:16">
       <c r="F56" t="s">
         <v>43</v>
       </c>
@@ -2994,8 +4756,20 @@
         <f t="shared" si="1"/>
         <v>2838</v>
       </c>
-    </row>
-    <row r="57" spans="6:12">
+      <c r="N56">
+        <f t="shared" si="2"/>
+        <v>166</v>
+      </c>
+      <c r="O56">
+        <f t="shared" si="3"/>
+        <v>2838</v>
+      </c>
+      <c r="P56">
+        <f t="shared" si="4"/>
+        <v>166</v>
+      </c>
+    </row>
+    <row r="57" spans="6:16">
       <c r="F57" t="s">
         <v>44</v>
       </c>
@@ -3013,8 +4787,20 @@
         <f t="shared" si="1"/>
         <v>2899</v>
       </c>
-    </row>
-    <row r="58" spans="6:12">
+      <c r="N57">
+        <f t="shared" si="2"/>
+        <v>160</v>
+      </c>
+      <c r="O57">
+        <f t="shared" si="3"/>
+        <v>2899</v>
+      </c>
+      <c r="P57">
+        <f t="shared" si="4"/>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="58" spans="6:16">
       <c r="F58" t="s">
         <v>45</v>
       </c>
@@ -3032,8 +4818,20 @@
         <f t="shared" si="1"/>
         <v>2960</v>
       </c>
-    </row>
-    <row r="59" spans="6:12">
+      <c r="N58">
+        <f t="shared" si="2"/>
+        <v>160</v>
+      </c>
+      <c r="O58">
+        <f t="shared" si="3"/>
+        <v>2960</v>
+      </c>
+      <c r="P58">
+        <f t="shared" si="4"/>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="59" spans="6:16">
       <c r="F59" t="s">
         <v>46</v>
       </c>
@@ -3051,8 +4849,20 @@
         <f t="shared" si="1"/>
         <v>3020</v>
       </c>
-    </row>
-    <row r="60" spans="6:12">
+      <c r="N59">
+        <f t="shared" si="2"/>
+        <v>148</v>
+      </c>
+      <c r="O59">
+        <f t="shared" si="3"/>
+        <v>3020</v>
+      </c>
+      <c r="P59">
+        <f t="shared" si="4"/>
+        <v>148</v>
+      </c>
+    </row>
+    <row r="60" spans="6:16">
       <c r="F60" t="s">
         <v>47</v>
       </c>
@@ -3070,8 +4880,20 @@
         <f t="shared" si="1"/>
         <v>3082</v>
       </c>
-    </row>
-    <row r="61" spans="6:12">
+      <c r="N60">
+        <f t="shared" si="2"/>
+        <v>146</v>
+      </c>
+      <c r="O60">
+        <f t="shared" si="3"/>
+        <v>3082</v>
+      </c>
+      <c r="P60">
+        <f t="shared" si="4"/>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="61" spans="6:16">
       <c r="F61" t="s">
         <v>48</v>
       </c>
@@ -3089,8 +4911,20 @@
         <f t="shared" si="1"/>
         <v>3142</v>
       </c>
-    </row>
-    <row r="62" spans="6:12">
+      <c r="N61">
+        <f t="shared" si="2"/>
+        <v>156</v>
+      </c>
+      <c r="O61">
+        <f t="shared" si="3"/>
+        <v>3142</v>
+      </c>
+      <c r="P61">
+        <f t="shared" si="4"/>
+        <v>156</v>
+      </c>
+    </row>
+    <row r="62" spans="6:16">
       <c r="F62" t="s">
         <v>49</v>
       </c>
@@ -3108,8 +4942,20 @@
         <f t="shared" si="1"/>
         <v>3202</v>
       </c>
-    </row>
-    <row r="63" spans="6:12">
+      <c r="N62">
+        <f t="shared" si="2"/>
+        <v>156</v>
+      </c>
+      <c r="O62">
+        <f t="shared" si="3"/>
+        <v>3202</v>
+      </c>
+      <c r="P62">
+        <f t="shared" si="4"/>
+        <v>156</v>
+      </c>
+    </row>
+    <row r="63" spans="6:16">
       <c r="F63" t="s">
         <v>50</v>
       </c>
@@ -3127,8 +4973,20 @@
         <f t="shared" si="1"/>
         <v>3264</v>
       </c>
-    </row>
-    <row r="64" spans="6:12">
+      <c r="N63">
+        <f t="shared" si="2"/>
+        <v>138</v>
+      </c>
+      <c r="O63">
+        <f t="shared" si="3"/>
+        <v>3264</v>
+      </c>
+      <c r="P63">
+        <f t="shared" si="4"/>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="64" spans="6:16">
       <c r="F64" t="s">
         <v>51</v>
       </c>
@@ -3146,8 +5004,20 @@
         <f t="shared" si="1"/>
         <v>3324</v>
       </c>
-    </row>
-    <row r="65" spans="6:12">
+      <c r="N64">
+        <f t="shared" si="2"/>
+        <v>160</v>
+      </c>
+      <c r="O64">
+        <f t="shared" si="3"/>
+        <v>3324</v>
+      </c>
+      <c r="P64">
+        <f t="shared" si="4"/>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="65" spans="6:16">
       <c r="F65" t="s">
         <v>52</v>
       </c>
@@ -3165,8 +5035,20 @@
         <f t="shared" si="1"/>
         <v>3385</v>
       </c>
-    </row>
-    <row r="66" spans="6:12">
+      <c r="N65">
+        <f t="shared" si="2"/>
+        <v>148</v>
+      </c>
+      <c r="O65">
+        <f t="shared" si="3"/>
+        <v>3385</v>
+      </c>
+      <c r="P65">
+        <f t="shared" si="4"/>
+        <v>148</v>
+      </c>
+    </row>
+    <row r="66" spans="6:16">
       <c r="F66" t="s">
         <v>53</v>
       </c>
@@ -3184,8 +5066,20 @@
         <f t="shared" si="1"/>
         <v>3446</v>
       </c>
-    </row>
-    <row r="67" spans="6:12">
+      <c r="N66">
+        <f t="shared" si="2"/>
+        <v>128</v>
+      </c>
+      <c r="O66">
+        <f t="shared" si="3"/>
+        <v>3446</v>
+      </c>
+      <c r="P66">
+        <f t="shared" si="4"/>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="67" spans="6:16">
       <c r="F67" t="s">
         <v>54</v>
       </c>
@@ -3203,8 +5097,20 @@
         <f t="shared" si="1"/>
         <v>3507</v>
       </c>
-    </row>
-    <row r="68" spans="6:12">
+      <c r="N67">
+        <f t="shared" si="2"/>
+        <v>136</v>
+      </c>
+      <c r="O67">
+        <f t="shared" si="3"/>
+        <v>3507</v>
+      </c>
+      <c r="P67">
+        <f t="shared" si="4"/>
+        <v>136</v>
+      </c>
+    </row>
+    <row r="68" spans="6:16">
       <c r="F68" t="s">
         <v>55</v>
       </c>
@@ -3222,8 +5128,20 @@
         <f t="shared" si="1"/>
         <v>3567</v>
       </c>
-    </row>
-    <row r="69" spans="6:12">
+      <c r="N68">
+        <f t="shared" si="2"/>
+        <v>136</v>
+      </c>
+      <c r="O68">
+        <f t="shared" si="3"/>
+        <v>3567</v>
+      </c>
+      <c r="P68">
+        <f t="shared" si="4"/>
+        <v>136</v>
+      </c>
+    </row>
+    <row r="69" spans="6:16">
       <c r="F69" t="s">
         <v>56</v>
       </c>
@@ -3241,8 +5159,20 @@
         <f t="shared" si="1"/>
         <v>3627</v>
       </c>
-    </row>
-    <row r="70" spans="6:12">
+      <c r="N69">
+        <f t="shared" si="2"/>
+        <v>124</v>
+      </c>
+      <c r="O69">
+        <f t="shared" si="3"/>
+        <v>3627</v>
+      </c>
+      <c r="P69">
+        <f t="shared" si="4"/>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="70" spans="6:16">
       <c r="F70" t="s">
         <v>57</v>
       </c>
@@ -3260,8 +5190,20 @@
         <f t="shared" si="1"/>
         <v>3689</v>
       </c>
-    </row>
-    <row r="71" spans="6:12">
+      <c r="N70">
+        <f t="shared" si="2"/>
+        <v>122</v>
+      </c>
+      <c r="O70">
+        <f t="shared" si="3"/>
+        <v>3689</v>
+      </c>
+      <c r="P70">
+        <f t="shared" si="4"/>
+        <v>122</v>
+      </c>
+    </row>
+    <row r="71" spans="6:16">
       <c r="F71" t="s">
         <v>58</v>
       </c>
@@ -3279,8 +5221,20 @@
         <f t="shared" si="1"/>
         <v>3749</v>
       </c>
-    </row>
-    <row r="72" spans="6:12">
+      <c r="N71">
+        <f t="shared" si="2"/>
+        <v>114</v>
+      </c>
+      <c r="O71">
+        <f t="shared" si="3"/>
+        <v>3749</v>
+      </c>
+      <c r="P71">
+        <f t="shared" si="4"/>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="72" spans="6:16">
       <c r="F72" t="s">
         <v>59</v>
       </c>

</xml_diff>